<commit_message>
Updating with new SIRFER data
</commit_message>
<xml_diff>
--- a/data/rawInterlabData.xlsx
+++ b/data/rawInterlabData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\GitHub\InterLabCompare\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933BB506-202F-4026-BF40-674119097DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBA2D04-BEEC-4BC4-8FF9-42096EB9AB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7320" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="33">
   <si>
     <t>sample</t>
   </si>
@@ -92,13 +92,40 @@
   </si>
   <si>
     <t>dpaa_treated_50</t>
+  </si>
+  <si>
+    <t>FE01</t>
+  </si>
+  <si>
+    <t>FE02</t>
+  </si>
+  <si>
+    <t>FE03</t>
+  </si>
+  <si>
+    <t>FE04</t>
+  </si>
+  <si>
+    <t>FE05</t>
+  </si>
+  <si>
+    <t>FE06</t>
+  </si>
+  <si>
+    <t>FE07</t>
+  </si>
+  <si>
+    <t>FE08</t>
+  </si>
+  <si>
+    <t>utah_untreated_30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -127,6 +154,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -570,10 +603,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103:C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1997,7 +2030,149 @@
         <v>-3.84</v>
       </c>
     </row>
+    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>14</v>
+      </c>
+      <c r="B102">
+        <v>-14.549566</v>
+      </c>
+      <c r="C102" t="s">
+        <v>32</v>
+      </c>
+      <c r="D102">
+        <v>-8.5316145999999993</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>24</v>
+      </c>
+      <c r="B103">
+        <v>-9.3290600000000001</v>
+      </c>
+      <c r="C103" t="s">
+        <v>32</v>
+      </c>
+      <c r="D103">
+        <v>-1.033345</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>25</v>
+      </c>
+      <c r="B104">
+        <v>-15.508796999999999</v>
+      </c>
+      <c r="C104" t="s">
+        <v>32</v>
+      </c>
+      <c r="D104">
+        <v>-7.5520424999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>26</v>
+      </c>
+      <c r="B105">
+        <v>-8.2918199999999995</v>
+      </c>
+      <c r="C105" t="s">
+        <v>32</v>
+      </c>
+      <c r="D105">
+        <v>-3.8960571000000002</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>27</v>
+      </c>
+      <c r="B106">
+        <v>-10.58713</v>
+      </c>
+      <c r="C106" t="s">
+        <v>32</v>
+      </c>
+      <c r="D106">
+        <v>-1.5984670999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>28</v>
+      </c>
+      <c r="B107">
+        <v>-15.971700999999999</v>
+      </c>
+      <c r="C107" t="s">
+        <v>32</v>
+      </c>
+      <c r="D107">
+        <v>-5.6693895999999997</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>29</v>
+      </c>
+      <c r="B108">
+        <v>-13.74333</v>
+      </c>
+      <c r="C108" t="s">
+        <v>32</v>
+      </c>
+      <c r="D108">
+        <v>-4.2283524999999997</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>30</v>
+      </c>
+      <c r="B109">
+        <v>-10.55585</v>
+      </c>
+      <c r="C109" t="s">
+        <v>32</v>
+      </c>
+      <c r="D109">
+        <v>0.5360066</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>31</v>
+      </c>
+      <c r="B110">
+        <v>-9.4439240000000009</v>
+      </c>
+      <c r="C110" t="s">
+        <v>32</v>
+      </c>
+      <c r="D110">
+        <v>-0.81820850000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111">
+        <v>-15.208564000000001</v>
+      </c>
+      <c r="C111" t="s">
+        <v>32</v>
+      </c>
+      <c r="D111">
+        <v>-8.2727003000000003</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>